<commit_message>
Finished v1.0 with bulk configuration generation.
</commit_message>
<xml_diff>
--- a/AirspanCIQ.xlsx
+++ b/AirspanCIQ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="9330"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="21600" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="PnpConfig" sheetId="1" r:id="rId1"/>
@@ -29,30 +29,6 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Windows User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-this is the eNB name</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -77,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="Y2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +61,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Windows User:</t>
         </r>
@@ -94,10 +70,58 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-this is the eNB name</t>
+IpRoute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IpRoute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IpRoute</t>
         </r>
       </text>
     </comment>
@@ -106,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -178,13 +202,91 @@
   </si>
   <si>
     <t>DataSubnetMask</t>
+  </si>
+  <si>
+    <t>DestIpAddress</t>
+  </si>
+  <si>
+    <t>IpSubnetMask</t>
+  </si>
+  <si>
+    <t>IpRouteList</t>
+  </si>
+  <si>
+    <t>DataIp</t>
+  </si>
+  <si>
+    <t>ControlIp</t>
+  </si>
+  <si>
+    <t>LTECell</t>
+  </si>
+  <si>
+    <t>PnpDetail/eNBDetail</t>
+  </si>
+  <si>
+    <t>GatewayIpAddress</t>
+  </si>
+  <si>
+    <t>WA-BEL01</t>
+  </si>
+  <si>
+    <t>Synergy2000</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>127.0.0.2</t>
+  </si>
+  <si>
+    <t>10.0.0.0</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
+  </si>
+  <si>
+    <t>124.0.0.0</t>
+  </si>
+  <si>
+    <t>124.0.0.1</t>
+  </si>
+  <si>
+    <t>196.0.0.0</t>
+  </si>
+  <si>
+    <t>196.0.0.1</t>
+  </si>
+  <si>
+    <t>WA-BEL03</t>
+  </si>
+  <si>
+    <t>WA-BEL02</t>
+  </si>
+  <si>
+    <t>127.0.0.3</t>
+  </si>
+  <si>
+    <t>128.0.0.1</t>
+  </si>
+  <si>
+    <t>128.0.0.2</t>
+  </si>
+  <si>
+    <t>128.0.0.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,16 +307,91 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -222,14 +399,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,22 +781,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -542,180 +812,187 @@
     <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="25"/>
+      <c r="W1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="23"/>
+    </row>
+    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X2" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>47.582467999999999</v>
+      </c>
+      <c r="D3">
+        <v>-122.136363</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>1001</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -738,35 +1015,274 @@
       <c r="O3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" s="1" t="s">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="U3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>47.582467999999999</v>
+      </c>
+      <c r="D4">
+        <v>-122.136363</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>1002</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>47.582467999999999</v>
+      </c>
+      <c r="D5">
+        <v>-122.136363</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5">
+        <v>1003</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="Y1:AG1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>